<commit_message>
second raund timesync and resampling corrections
</commit_message>
<xml_diff>
--- a/Data/livinglabUsersFileFolderNames.xlsx
+++ b/Data/livinglabUsersFileFolderNames.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="266">
   <si>
     <t>uID</t>
   </si>
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>user50/Tobii/</t>
+  </si>
+  <si>
+    <t>user5/Tobii/</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1148,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,10 +2237,10 @@
         <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>265</v>
       </c>
       <c r="H40" t="s">
-        <v>194</v>
+        <v>265</v>
       </c>
       <c r="I40">
         <v>1</v>

</xml_diff>